<commit_message>
files with code for schools
</commit_message>
<xml_diff>
--- a/Data/measles_TX_02_28_2025.xlsx
+++ b/Data/measles_TX_02_28_2025.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jh56833/Documents/GitHub/Measles_in_Texas/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419F443E-333E-2646-A2B5-E72CD4235C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{158CC2FE-945A-AB40-9BA7-FFB0F3C10358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{E44F9C15-D4D8-1546-8A8F-227CD7E6AAAD}"/>
+    <workbookView xWindow="-51200" yWindow="-5440" windowWidth="51200" windowHeight="27160" activeTab="1" xr2:uid="{E44F9C15-D4D8-1546-8A8F-227CD7E6AAAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="24">
   <si>
     <t>County</t>
   </si>
@@ -75,13 +76,46 @@
   </si>
   <si>
     <t>As_of</t>
+  </si>
+  <si>
+    <t>Cochran</t>
+  </si>
+  <si>
+    <t>Lamar</t>
+  </si>
+  <si>
+    <t>as of Mar 14 2025</t>
+  </si>
+  <si>
+    <t>as_of</t>
+  </si>
+  <si>
+    <t>Diff_previous</t>
+  </si>
+  <si>
+    <t>as of March 18</t>
+  </si>
+  <si>
+    <t>Garza</t>
+  </si>
+  <si>
+    <t>Hale</t>
+  </si>
+  <si>
+    <t>Hockley</t>
+  </si>
+  <si>
+    <t>Lamb</t>
+  </si>
+  <si>
+    <t>as of Mar 25 2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,6 +147,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -134,12 +174,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +515,621 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EB1ABB-0803-9F48-8DF7-FCBC6EDCB718}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:R16"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="5">
+        <f t="shared" ref="I2:I12" si="0">100*(F2-B2)/F2</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1">
+        <v>6</v>
+      </c>
+      <c r="M2" t="s">
+        <v>18</v>
+      </c>
+      <c r="N2" s="5">
+        <f>100*(L2-F2)/L2</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>6</v>
+      </c>
+      <c r="R2" s="5">
+        <f>(Q2-L2)*L2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="5">
+        <f t="shared" si="0"/>
+        <v>27.272727272727273</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="5">
+        <f t="shared" ref="N3:N12" si="1">100*(L3-F3)/L3</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>13</v>
+      </c>
+      <c r="R3" s="5">
+        <f t="shared" ref="R3:R16" si="2">(Q3-L3)*L3</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>2</v>
+      </c>
+      <c r="R4" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1">
+        <v>174</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="0"/>
+        <v>43.678160919540232</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>191</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" si="1"/>
+        <v>8.9005235602094235</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>226</v>
+      </c>
+      <c r="R5" s="5">
+        <f t="shared" si="2"/>
+        <v>6685</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>4</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N6" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>10</v>
+      </c>
+      <c r="R6" s="5">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>1</v>
+      </c>
+      <c r="R7" s="5">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="1">
+        <v>3</v>
+      </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>3</v>
+      </c>
+      <c r="R8" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="1">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="0"/>
+        <v>41.666666666666664</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="1">
+        <v>36</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>37</v>
+      </c>
+      <c r="R9" s="5">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1">
+        <v>11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="0"/>
+        <v>45.454545454545453</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="1">
+        <v>11</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N10" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>13</v>
+      </c>
+      <c r="R10" s="5">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="1">
+        <v>7</v>
+      </c>
+      <c r="M11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N11" s="5">
+        <f t="shared" si="1"/>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>7</v>
+      </c>
+      <c r="R11" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4</v>
+      </c>
+      <c r="G12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="1">
+        <v>5</v>
+      </c>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="5">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>5</v>
+      </c>
+      <c r="R12" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="P13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>1</v>
+      </c>
+      <c r="R13" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="P14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>1</v>
+      </c>
+      <c r="R14" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="P15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>1</v>
+      </c>
+      <c r="R15" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="P16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>1</v>
+      </c>
+      <c r="R16" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{934DBB4C-76C1-9744-B843-8704D5553410}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -490,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -498,10 +1150,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -509,10 +1161,10 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -523,7 +1175,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -531,10 +1183,10 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>98</v>
+        <v>226</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -542,10 +1194,10 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -553,10 +1205,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -567,7 +1219,7 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -575,10 +1227,10 @@
         <v>9</v>
       </c>
       <c r="B9" s="1">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -586,17 +1238,80 @@
         <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>